<commit_message>
logging problems solved, fixed bugs
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BC6"/>
+  <dimension ref="A1:BC9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -711,18 +711,28 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>as asdasdas sad</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>123</v>
+      </c>
       <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>28-08-2023</t>
+          <t>29-08-2023</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:08</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
@@ -730,120 +740,375 @@
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
+      <c r="L2" t="n">
+        <v>7</v>
+      </c>
+      <c r="M2" t="n">
+        <v>5</v>
+      </c>
+      <c r="N2" t="n">
+        <v>5</v>
+      </c>
+      <c r="O2" t="n">
+        <v>2</v>
+      </c>
+      <c r="P2" t="n">
+        <v>3</v>
+      </c>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr"/>
       <c r="U2" t="inlineStr"/>
-      <c r="V2" t="inlineStr"/>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">qwe
+</t>
+        </is>
+      </c>
       <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr"/>
       <c r="Y2" t="inlineStr"/>
       <c r="Z2" t="inlineStr"/>
       <c r="AA2" t="inlineStr"/>
-      <c r="AB2" t="inlineStr"/>
-      <c r="AC2" t="inlineStr"/>
-      <c r="AD2" t="inlineStr"/>
-      <c r="AE2" t="inlineStr"/>
-      <c r="AF2" t="inlineStr"/>
-      <c r="AG2" t="inlineStr"/>
+      <c r="AB2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>6</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1-2 недели
+</t>
+        </is>
+      </c>
       <c r="AH2" t="inlineStr"/>
       <c r="AI2" t="inlineStr"/>
       <c r="AJ2" t="inlineStr"/>
       <c r="AK2" t="inlineStr"/>
-      <c r="AL2" t="inlineStr"/>
+      <c r="AL2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">qwe
+</t>
+        </is>
+      </c>
       <c r="AM2" t="inlineStr"/>
       <c r="AN2" t="inlineStr"/>
       <c r="AO2" t="inlineStr"/>
       <c r="AP2" t="inlineStr"/>
       <c r="AQ2" t="inlineStr"/>
-      <c r="AR2" t="inlineStr"/>
-      <c r="AS2" t="inlineStr"/>
-      <c r="AT2" t="inlineStr"/>
-      <c r="AU2" t="inlineStr"/>
-      <c r="AV2" t="inlineStr"/>
+      <c r="AR2" t="n">
+        <v>18</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>16</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>15</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>15</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>16</v>
+      </c>
       <c r="AW2" t="inlineStr"/>
       <c r="AX2" t="inlineStr"/>
       <c r="AY2" t="inlineStr"/>
       <c r="AZ2" t="inlineStr"/>
       <c r="BA2" t="inlineStr"/>
-      <c r="BB2" t="inlineStr"/>
-      <c r="BC2" t="inlineStr"/>
+      <c r="BB2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">asd
+</t>
+        </is>
+      </c>
+      <c r="BC2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">qwe
+</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>assd asd asdqw e</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>123</v>
+      </c>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>asdxcas</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>28-08-2023</t>
+          <t>29-08-2023</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>21:20</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
+          <t>21:10</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ЙЦУК
+</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">фыв
+</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ячс
+</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">фыв
+</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">фыв
+</t>
+        </is>
+      </c>
+      <c r="L3" t="n">
+        <v>9</v>
+      </c>
+      <c r="M3" t="n">
+        <v>7</v>
+      </c>
+      <c r="N3" t="n">
+        <v>6</v>
+      </c>
+      <c r="O3" t="n">
+        <v>5</v>
+      </c>
+      <c r="P3" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3 дня
+</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1-2 недели
+</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4 месяца
+</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4 месяца
+</t>
+        </is>
+      </c>
       <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr">
         <is>
-          <t>
-</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="inlineStr"/>
-      <c r="Z3" t="inlineStr"/>
-      <c r="AA3" t="inlineStr"/>
-      <c r="AB3" t="inlineStr"/>
-      <c r="AC3" t="inlineStr"/>
-      <c r="AD3" t="inlineStr"/>
-      <c r="AE3" t="inlineStr"/>
-      <c r="AF3" t="inlineStr"/>
-      <c r="AG3" t="inlineStr"/>
-      <c r="AH3" t="inlineStr"/>
-      <c r="AI3" t="inlineStr"/>
-      <c r="AJ3" t="inlineStr"/>
-      <c r="AK3" t="inlineStr"/>
-      <c r="AL3" t="inlineStr"/>
-      <c r="AM3" t="inlineStr"/>
-      <c r="AN3" t="inlineStr"/>
-      <c r="AO3" t="inlineStr"/>
-      <c r="AP3" t="inlineStr"/>
-      <c r="AQ3" t="inlineStr"/>
-      <c r="AR3" t="inlineStr"/>
-      <c r="AS3" t="inlineStr"/>
-      <c r="AT3" t="inlineStr"/>
-      <c r="AU3" t="inlineStr"/>
-      <c r="AV3" t="inlineStr"/>
-      <c r="AW3" t="inlineStr"/>
-      <c r="AX3" t="inlineStr"/>
-      <c r="AY3" t="inlineStr"/>
-      <c r="AZ3" t="inlineStr"/>
-      <c r="BA3" t="inlineStr"/>
-      <c r="BB3" t="inlineStr"/>
-      <c r="BC3" t="inlineStr"/>
+          <t xml:space="preserve">asd
+</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">фыв
+</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">фыв
+</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">фыв
+</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">фыв
+</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ячс
+</t>
+        </is>
+      </c>
+      <c r="AB3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1-2 недели
+</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4 месяца
+</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3 дня
+</t>
+        </is>
+      </c>
+      <c r="AJ3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4 месяца
+</t>
+        </is>
+      </c>
+      <c r="AK3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3 дня
+</t>
+        </is>
+      </c>
+      <c r="AL3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">asd
+</t>
+        </is>
+      </c>
+      <c r="AM3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">фыв
+</t>
+        </is>
+      </c>
+      <c r="AN3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">фыв
+</t>
+        </is>
+      </c>
+      <c r="AO3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ЙЦУК
+</t>
+        </is>
+      </c>
+      <c r="AP3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ЙЦУК
+</t>
+        </is>
+      </c>
+      <c r="AQ3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">фыв
+</t>
+        </is>
+      </c>
+      <c r="AR3" t="n">
+        <v>17</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>16</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>15</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>16</v>
+      </c>
+      <c r="AV3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AW3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1-2 недели
+</t>
+        </is>
+      </c>
+      <c r="AX3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1-2 недели
+</t>
+        </is>
+      </c>
+      <c r="AY3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3 дня
+</t>
+        </is>
+      </c>
+      <c r="AZ3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3 дня
+</t>
+        </is>
+      </c>
+      <c r="BA3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1-2 недели
+</t>
+        </is>
+      </c>
+      <c r="BB3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">asd
+</t>
+        </is>
+      </c>
+      <c r="BC3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">asd
+</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -852,27 +1117,17 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>28-08-2023</t>
+          <t>29-08-2023</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:15</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ЙЦУК
-</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">фыв
-</t>
-        </is>
-      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
@@ -880,10 +1135,30 @@
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3 дня
+</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1-2 недели
+</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4 месяца
+</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4 месяца
+</t>
+        </is>
+      </c>
       <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr">
         <is>
@@ -906,7 +1181,12 @@
       <c r="AI4" t="inlineStr"/>
       <c r="AJ4" t="inlineStr"/>
       <c r="AK4" t="inlineStr"/>
-      <c r="AL4" t="inlineStr"/>
+      <c r="AL4" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
       <c r="AM4" t="inlineStr"/>
       <c r="AN4" t="inlineStr"/>
       <c r="AO4" t="inlineStr"/>
@@ -922,30 +1202,32 @@
       <c r="AY4" t="inlineStr"/>
       <c r="AZ4" t="inlineStr"/>
       <c r="BA4" t="inlineStr"/>
-      <c r="BB4" t="inlineStr"/>
-      <c r="BC4" t="inlineStr"/>
+      <c r="BB4" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+      <c r="BC4" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>qwe</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>28-08-2023</t>
+          <t>29-08-2023</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>21:18</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
@@ -958,12 +1240,37 @@
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr"/>
-      <c r="T5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3 дня
+</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1-2 недели
+</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4 месяца
+</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4 месяца
+</t>
+        </is>
+      </c>
       <c r="U5" t="inlineStr"/>
-      <c r="V5" t="inlineStr"/>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
       <c r="W5" t="inlineStr"/>
       <c r="X5" t="inlineStr"/>
       <c r="Y5" t="inlineStr"/>
@@ -979,7 +1286,12 @@
       <c r="AI5" t="inlineStr"/>
       <c r="AJ5" t="inlineStr"/>
       <c r="AK5" t="inlineStr"/>
-      <c r="AL5" t="inlineStr"/>
+      <c r="AL5" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
       <c r="AM5" t="inlineStr"/>
       <c r="AN5" t="inlineStr"/>
       <c r="AO5" t="inlineStr"/>
@@ -995,102 +1307,760 @@
       <c r="AY5" t="inlineStr"/>
       <c r="AZ5" t="inlineStr"/>
       <c r="BA5" t="inlineStr"/>
-      <c r="BB5" t="inlineStr"/>
-      <c r="BC5" t="inlineStr"/>
+      <c r="BB5" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+      <c r="BC5" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>qwe</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>qwe</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
+          <t xml:space="preserve">asd asd asd </t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>123123</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Коля
+</t>
+        </is>
+      </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>qwe</t>
+          <t>qweqwe</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>28-08-2023</t>
+          <t>29-08-2023</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>22:29</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr"/>
-      <c r="S6" t="inlineStr"/>
-      <c r="T6" t="inlineStr"/>
-      <c r="U6" t="inlineStr"/>
+          <t>21:19</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ЙЦУК
+</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">фыв
+</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">фыв
+</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">фыв
+</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">фыв
+</t>
+        </is>
+      </c>
+      <c r="L6" t="n">
+        <v>3</v>
+      </c>
+      <c r="M6" t="n">
+        <v>3</v>
+      </c>
+      <c r="N6" t="n">
+        <v>2</v>
+      </c>
+      <c r="O6" t="n">
+        <v>1</v>
+      </c>
+      <c r="P6" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3 дня
+</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1-2 недели
+</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1-2 недели
+</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1-2 недели
+</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3 дня
+</t>
+        </is>
+      </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t xml:space="preserve">qwe
-</t>
-        </is>
-      </c>
-      <c r="W6" t="inlineStr"/>
-      <c r="X6" t="inlineStr"/>
-      <c r="Y6" t="inlineStr"/>
-      <c r="Z6" t="inlineStr"/>
-      <c r="AA6" t="inlineStr"/>
-      <c r="AB6" t="inlineStr"/>
-      <c r="AC6" t="inlineStr"/>
-      <c r="AD6" t="inlineStr"/>
-      <c r="AE6" t="inlineStr"/>
-      <c r="AF6" t="inlineStr"/>
-      <c r="AG6" t="inlineStr"/>
-      <c r="AH6" t="inlineStr"/>
-      <c r="AI6" t="inlineStr"/>
-      <c r="AJ6" t="inlineStr"/>
-      <c r="AK6" t="inlineStr"/>
+          <t xml:space="preserve">asd
+</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ЙЦУК
+</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ЙЦУК
+</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">фыв
+</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">фыв
+</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">фыв
+</t>
+        </is>
+      </c>
+      <c r="AB6" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>7</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1-2 недели
+</t>
+        </is>
+      </c>
+      <c r="AH6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1-2 недели
+</t>
+        </is>
+      </c>
+      <c r="AI6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1-2 недели
+</t>
+        </is>
+      </c>
+      <c r="AJ6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3 дня
+</t>
+        </is>
+      </c>
+      <c r="AK6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3 дня
+</t>
+        </is>
+      </c>
       <c r="AL6" t="inlineStr">
         <is>
-          <t xml:space="preserve">qwe
-</t>
-        </is>
-      </c>
-      <c r="AM6" t="inlineStr"/>
-      <c r="AN6" t="inlineStr"/>
-      <c r="AO6" t="inlineStr"/>
-      <c r="AP6" t="inlineStr"/>
-      <c r="AQ6" t="inlineStr"/>
-      <c r="AR6" t="inlineStr"/>
-      <c r="AS6" t="inlineStr"/>
-      <c r="AT6" t="inlineStr"/>
-      <c r="AU6" t="inlineStr"/>
-      <c r="AV6" t="inlineStr"/>
-      <c r="AW6" t="inlineStr"/>
-      <c r="AX6" t="inlineStr"/>
-      <c r="AY6" t="inlineStr"/>
-      <c r="AZ6" t="inlineStr"/>
-      <c r="BA6" t="inlineStr"/>
+          <t xml:space="preserve">asd
+</t>
+        </is>
+      </c>
+      <c r="AM6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ЙЦУК
+</t>
+        </is>
+      </c>
+      <c r="AN6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">фыв
+</t>
+        </is>
+      </c>
+      <c r="AO6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">фыв
+</t>
+        </is>
+      </c>
+      <c r="AP6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">фыв
+</t>
+        </is>
+      </c>
+      <c r="AQ6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ЙЦУК
+</t>
+        </is>
+      </c>
+      <c r="AR6" t="n">
+        <v>13</v>
+      </c>
+      <c r="AS6" t="n">
+        <v>15</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>13</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>14</v>
+      </c>
+      <c r="AV6" t="n">
+        <v>17</v>
+      </c>
+      <c r="AW6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1-2 недели
+</t>
+        </is>
+      </c>
+      <c r="AX6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3 дня
+</t>
+        </is>
+      </c>
+      <c r="AY6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3 дня
+</t>
+        </is>
+      </c>
+      <c r="AZ6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1-2 недели
+</t>
+        </is>
+      </c>
+      <c r="BA6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4 месяца
+</t>
+        </is>
+      </c>
       <c r="BB6" t="inlineStr">
         <is>
-          <t xml:space="preserve">qwe
+          <t xml:space="preserve">asd
 </t>
         </is>
       </c>
       <c r="BC6" t="inlineStr">
         <is>
-          <t xml:space="preserve">qwe
+          <t xml:space="preserve">asd
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">asd asd asd </t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>123123</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Коля
+</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>qweqwe</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>29-08-2023</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ЙЦУК
+</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">фыв
+</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">фыв
+</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">фыв
+</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">фыв
+</t>
+        </is>
+      </c>
+      <c r="L7" t="n">
+        <v>3</v>
+      </c>
+      <c r="M7" t="n">
+        <v>3</v>
+      </c>
+      <c r="N7" t="n">
+        <v>2</v>
+      </c>
+      <c r="O7" t="n">
+        <v>1</v>
+      </c>
+      <c r="P7" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3 дня
+</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1-2 недели
+</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1-2 недели
+</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1-2 недели
+</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3 дня
+</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">asd
+</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ЙЦУК
+</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ЙЦУК
+</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">фыв
+</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">фыв
+</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">фыв
+</t>
+        </is>
+      </c>
+      <c r="AB7" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>7</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1-2 недели
+</t>
+        </is>
+      </c>
+      <c r="AH7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1-2 недели
+</t>
+        </is>
+      </c>
+      <c r="AI7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1-2 недели
+</t>
+        </is>
+      </c>
+      <c r="AJ7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3 дня
+</t>
+        </is>
+      </c>
+      <c r="AK7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3 дня
+</t>
+        </is>
+      </c>
+      <c r="AL7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">asd
+</t>
+        </is>
+      </c>
+      <c r="AM7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ЙЦУК
+</t>
+        </is>
+      </c>
+      <c r="AN7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">фыв
+</t>
+        </is>
+      </c>
+      <c r="AO7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">фыв
+</t>
+        </is>
+      </c>
+      <c r="AP7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">фыв
+</t>
+        </is>
+      </c>
+      <c r="AQ7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ЙЦУК
+</t>
+        </is>
+      </c>
+      <c r="AR7" t="n">
+        <v>13</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>15</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>13</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>14</v>
+      </c>
+      <c r="AV7" t="n">
+        <v>17</v>
+      </c>
+      <c r="AW7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1-2 недели
+</t>
+        </is>
+      </c>
+      <c r="AX7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3 дня
+</t>
+        </is>
+      </c>
+      <c r="AY7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3 дня
+</t>
+        </is>
+      </c>
+      <c r="AZ7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1-2 недели
+</t>
+        </is>
+      </c>
+      <c r="BA7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4 месяца
+</t>
+        </is>
+      </c>
+      <c r="BB7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">asd
+</t>
+        </is>
+      </c>
+      <c r="BC7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">asd
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>asdasd asdasd asd</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>123</v>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>qsw</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>29-08-2023</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>21:22</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr"/>
+      <c r="X8" t="inlineStr"/>
+      <c r="Y8" t="inlineStr"/>
+      <c r="Z8" t="inlineStr"/>
+      <c r="AA8" t="inlineStr"/>
+      <c r="AB8" t="inlineStr"/>
+      <c r="AC8" t="inlineStr"/>
+      <c r="AD8" t="inlineStr"/>
+      <c r="AE8" t="inlineStr"/>
+      <c r="AF8" t="inlineStr"/>
+      <c r="AG8" t="inlineStr"/>
+      <c r="AH8" t="inlineStr"/>
+      <c r="AI8" t="inlineStr"/>
+      <c r="AJ8" t="inlineStr"/>
+      <c r="AK8" t="inlineStr"/>
+      <c r="AL8" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+      <c r="AM8" t="inlineStr"/>
+      <c r="AN8" t="inlineStr"/>
+      <c r="AO8" t="inlineStr"/>
+      <c r="AP8" t="inlineStr"/>
+      <c r="AQ8" t="inlineStr"/>
+      <c r="AR8" t="inlineStr"/>
+      <c r="AS8" t="inlineStr"/>
+      <c r="AT8" t="inlineStr"/>
+      <c r="AU8" t="inlineStr"/>
+      <c r="AV8" t="inlineStr"/>
+      <c r="AW8" t="inlineStr"/>
+      <c r="AX8" t="inlineStr"/>
+      <c r="AY8" t="inlineStr"/>
+      <c r="AZ8" t="inlineStr"/>
+      <c r="BA8" t="inlineStr"/>
+      <c r="BB8" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+      <c r="BC8" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Коля
+</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>29-08-2023</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>21:26</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr"/>
+      <c r="X9" t="inlineStr"/>
+      <c r="Y9" t="inlineStr"/>
+      <c r="Z9" t="inlineStr"/>
+      <c r="AA9" t="inlineStr"/>
+      <c r="AB9" t="inlineStr"/>
+      <c r="AC9" t="inlineStr"/>
+      <c r="AD9" t="inlineStr"/>
+      <c r="AE9" t="inlineStr"/>
+      <c r="AF9" t="inlineStr"/>
+      <c r="AG9" t="inlineStr"/>
+      <c r="AH9" t="inlineStr"/>
+      <c r="AI9" t="inlineStr"/>
+      <c r="AJ9" t="inlineStr"/>
+      <c r="AK9" t="inlineStr"/>
+      <c r="AL9" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+      <c r="AM9" t="inlineStr"/>
+      <c r="AN9" t="inlineStr"/>
+      <c r="AO9" t="inlineStr"/>
+      <c r="AP9" t="inlineStr"/>
+      <c r="AQ9" t="inlineStr"/>
+      <c r="AR9" t="inlineStr"/>
+      <c r="AS9" t="inlineStr"/>
+      <c r="AT9" t="inlineStr"/>
+      <c r="AU9" t="inlineStr"/>
+      <c r="AV9" t="inlineStr"/>
+      <c r="AW9" t="inlineStr"/>
+      <c r="AX9" t="inlineStr"/>
+      <c r="AY9" t="inlineStr"/>
+      <c r="AZ9" t="inlineStr"/>
+      <c r="BA9" t="inlineStr"/>
+      <c r="BB9" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+      <c r="BC9" t="inlineStr">
+        <is>
+          <t>
 </t>
         </is>
       </c>

</xml_diff>